<commit_message>
Consolidate number of courses
</commit_message>
<xml_diff>
--- a/data/Poly 2023 LAS Reference.xlsx
+++ b/data/Poly 2023 LAS Reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chooyen\myenv\streamlit_apps\streamlit-Course Selection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDE388F-2C04-437C-BDC5-E5747E19A042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44632ACF-0FB0-46C7-9DE9-FF3AA871E597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RP" sheetId="12" r:id="rId1"/>
@@ -40,9 +40,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="445">
   <si>
-    <t xml:space="preserve">MOE Course Code </t>
-  </si>
-  <si>
     <t>T26</t>
   </si>
   <si>
@@ -892,9 +889,6 @@
     <t>CHEMICAL &amp; BIOMOLECULAR ENGINEERING</t>
   </si>
   <si>
-    <t xml:space="preserve">Course Name </t>
-  </si>
-  <si>
     <t>S30</t>
   </si>
   <si>
@@ -1345,9 +1339,6 @@
     <t>10-25</t>
   </si>
   <si>
-    <t xml:space="preserve">Aggregate Type </t>
-  </si>
-  <si>
     <t>ELR2B2-C</t>
   </si>
   <si>
@@ -1373,6 +1364,15 @@
   </si>
   <si>
     <t xml:space="preserve">CYBERSECURITY &amp; DIGITAL FORENSICS* </t>
+  </si>
+  <si>
+    <t>MOE Course Code</t>
+  </si>
+  <si>
+    <t>Course Name</t>
+  </si>
+  <si>
+    <t>Aggregate Type</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1797,7 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1812,618 +1812,618 @@
   <sheetData>
     <row r="1" spans="1:4" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>442</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>284</v>
+        <v>443</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>275</v>
-      </c>
       <c r="C4" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>267</v>
-      </c>
       <c r="C9" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>242</v>
-      </c>
       <c r="C16" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>236</v>
-      </c>
       <c r="C17" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="B19" s="21" t="s">
-        <v>228</v>
-      </c>
       <c r="C19" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="B22" s="21" t="s">
-        <v>256</v>
-      </c>
       <c r="C22" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>254</v>
-      </c>
       <c r="C23" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="B26" s="21" t="s">
-        <v>260</v>
-      </c>
       <c r="C26" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>262</v>
-      </c>
       <c r="C27" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="B28" s="21" t="s">
-        <v>238</v>
-      </c>
       <c r="C28" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="B30" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="B30" s="21" t="s">
-        <v>246</v>
-      </c>
       <c r="C30" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="B33" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>232</v>
-      </c>
       <c r="C33" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B35" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="B35" s="21" t="s">
-        <v>273</v>
-      </c>
       <c r="C35" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B36" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="B36" s="21" t="s">
-        <v>234</v>
-      </c>
       <c r="C36" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="B38" s="21" t="s">
-        <v>240</v>
-      </c>
       <c r="C38" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="B39" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="B39" s="21" t="s">
-        <v>278</v>
-      </c>
       <c r="C39" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="B40" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="B40" s="21" t="s">
-        <v>258</v>
-      </c>
       <c r="C40" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B41" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="B41" s="21" t="s">
-        <v>264</v>
-      </c>
       <c r="C41" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="B42" s="21" t="s">
-        <v>248</v>
-      </c>
       <c r="C42" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -2443,7 +2443,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2457,576 +2457,576 @@
   <sheetData>
     <row r="1" spans="1:4" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>442</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>284</v>
+        <v>443</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>158</v>
-      </c>
       <c r="C4" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>160</v>
-      </c>
       <c r="C5" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="C10" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>180</v>
-      </c>
       <c r="C12" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>151</v>
-      </c>
       <c r="C14" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>147</v>
-      </c>
       <c r="C15" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>135</v>
-      </c>
       <c r="C16" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B25" s="21" t="s">
-        <v>153</v>
-      </c>
       <c r="C25" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>140</v>
-      </c>
       <c r="C27" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="B28" s="21" t="s">
-        <v>133</v>
-      </c>
       <c r="C28" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="B29" s="21" t="s">
-        <v>175</v>
-      </c>
       <c r="C29" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="B32" s="21" t="s">
-        <v>177</v>
-      </c>
       <c r="C32" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="21" t="s">
-        <v>145</v>
-      </c>
       <c r="C34" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="21" t="s">
-        <v>156</v>
-      </c>
       <c r="C35" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="B37" s="21" t="s">
-        <v>169</v>
-      </c>
       <c r="C37" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="B39" s="21" t="s">
-        <v>165</v>
-      </c>
       <c r="C39" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="21" t="s">
-        <v>143</v>
-      </c>
       <c r="C41" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3046,7 +3046,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3060,478 +3060,478 @@
   <sheetData>
     <row r="1" spans="1:4" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>442</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>284</v>
+        <v>443</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>210</v>
-      </c>
       <c r="C3" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>186</v>
-      </c>
       <c r="C6" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>201</v>
-      </c>
       <c r="C10" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="B19" s="21" t="s">
-        <v>214</v>
-      </c>
       <c r="C19" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>193</v>
-      </c>
       <c r="C21" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="B22" s="21" t="s">
-        <v>184</v>
-      </c>
       <c r="C22" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>199</v>
-      </c>
       <c r="C23" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="B25" s="21" t="s">
-        <v>190</v>
-      </c>
       <c r="C25" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="B26" s="21" t="s">
-        <v>225</v>
-      </c>
       <c r="C26" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>196</v>
-      </c>
       <c r="C27" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="B28" s="21" t="s">
-        <v>221</v>
-      </c>
       <c r="C28" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="B29" s="21" t="s">
-        <v>223</v>
-      </c>
       <c r="C29" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="B31" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B31" s="21" t="s">
-        <v>208</v>
-      </c>
       <c r="C31" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B34" s="21" t="s">
-        <v>182</v>
-      </c>
       <c r="C34" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3543,7 +3543,7 @@
     <row r="36" spans="1:4" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="17" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="14"/>
@@ -3564,8 +3564,8 @@
   </sheetPr>
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3579,590 +3579,590 @@
   <sheetData>
     <row r="1" spans="1:4" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>442</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>284</v>
+        <v>443</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>283</v>
-      </c>
       <c r="C9" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4174,7 +4174,7 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="15" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C44" s="16"/>
       <c r="D44" s="14"/>
@@ -4195,8 +4195,8 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -4211,590 +4211,590 @@
   <sheetData>
     <row r="1" spans="1:4" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>442</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>284</v>
+        <v>443</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>